<commit_message>
Finishing Latex and extra figures in R
</commit_message>
<xml_diff>
--- a/Behavior Tables.xlsx
+++ b/Behavior Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Regressions" sheetId="1" r:id="rId1"/>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="213">
   <si>
     <t>slope</t>
   </si>
@@ -457,15 +457,283 @@
   </si>
   <si>
     <t>21.8(12.6)</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Direction</t>
+  </si>
+  <si>
+    <t>Latency (SD) during leftward movements</t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t>96.6 (20.6)</t>
+  </si>
+  <si>
+    <t>238.9 (54.0)</t>
+  </si>
+  <si>
+    <t>246.6 (43.0)</t>
+  </si>
+  <si>
+    <t>96.2 (20.0)</t>
+  </si>
+  <si>
+    <t>244.4 (56.1)</t>
+  </si>
+  <si>
+    <t>254.4 (59.7)</t>
+  </si>
+  <si>
+    <t>95.9 (20.0)</t>
+  </si>
+  <si>
+    <t>187.0 (21.2)</t>
+  </si>
+  <si>
+    <t>93.7 (16.5)</t>
+  </si>
+  <si>
+    <t>216.1 (48.9)</t>
+  </si>
+  <si>
+    <t>257.5 (59.0)</t>
+  </si>
+  <si>
+    <t>95.4 (18.1)</t>
+  </si>
+  <si>
+    <t>238.9 (52.3)</t>
+  </si>
+  <si>
+    <t>224.2 (34.0)</t>
+  </si>
+  <si>
+    <t>95.5 (18.5)</t>
+  </si>
+  <si>
+    <t>253.7 (58.5)</t>
+  </si>
+  <si>
+    <t>200.7 (25.5)</t>
+  </si>
+  <si>
+    <t>103.8 (21.7)</t>
+  </si>
+  <si>
+    <t>202.9 (43.7)</t>
+  </si>
+  <si>
+    <t>247.6 (52.1)</t>
+  </si>
+  <si>
+    <t>105.8 (22.8)</t>
+  </si>
+  <si>
+    <t>211.4 (44.0)</t>
+  </si>
+  <si>
+    <t>220.2 (38.9)</t>
+  </si>
+  <si>
+    <t>105.5 (22.5)</t>
+  </si>
+  <si>
+    <t>220.2 (39.9)</t>
+  </si>
+  <si>
+    <t>204.6 (31.4)</t>
+  </si>
+  <si>
+    <t>100.9 (19.7)</t>
+  </si>
+  <si>
+    <t>212.2 (41.4)</t>
+  </si>
+  <si>
+    <t>215.5 (41.7)</t>
+  </si>
+  <si>
+    <t>101.5 (20.1)</t>
+  </si>
+  <si>
+    <t>228.1 (44.9)</t>
+  </si>
+  <si>
+    <t>210.3 (33.2)</t>
+  </si>
+  <si>
+    <t>100.7 (19.6)</t>
+  </si>
+  <si>
+    <t>251.8 (51.2)</t>
+  </si>
+  <si>
+    <t>204.7 (27.8)</t>
+  </si>
+  <si>
+    <t>98.1 (23.5)</t>
+  </si>
+  <si>
+    <t>94.4 (19.6)</t>
+  </si>
+  <si>
+    <t>121.1 (38.3)</t>
+  </si>
+  <si>
+    <t>97.8 (24.2)</t>
+  </si>
+  <si>
+    <t>91.4 (14.8)</t>
+  </si>
+  <si>
+    <t>113.8 (30.8)</t>
+  </si>
+  <si>
+    <t>115.2 (27.1)</t>
+  </si>
+  <si>
+    <t>109.2 (21.7)</t>
+  </si>
+  <si>
+    <t>141.9 (41.1)</t>
+  </si>
+  <si>
+    <t>114.7 (26.9)</t>
+  </si>
+  <si>
+    <t>106.9 (24.3)</t>
+  </si>
+  <si>
+    <t>142.0 (47.0)</t>
+  </si>
+  <si>
+    <t>221.4 (71.8)</t>
+  </si>
+  <si>
+    <t>251.8 (59.5)</t>
+  </si>
+  <si>
+    <t>316.2 (85.5)</t>
+  </si>
+  <si>
+    <t>238.1 (52.9)</t>
+  </si>
+  <si>
+    <t>217.2 (31.3)</t>
+  </si>
+  <si>
+    <t>248.8 (61.2)</t>
+  </si>
+  <si>
+    <t>217.4 (38.3)</t>
+  </si>
+  <si>
+    <t>208.2 (32.0)</t>
+  </si>
+  <si>
+    <t>261.9 (69.5)</t>
+  </si>
+  <si>
+    <t>218.3 (26.3)</t>
+  </si>
+  <si>
+    <t>229.1 (33.6)</t>
+  </si>
+  <si>
+    <t>242.9 (30.4)</t>
+  </si>
+  <si>
+    <t>230.8 (26.5)</t>
+  </si>
+  <si>
+    <t>201.2 (25.2)</t>
+  </si>
+  <si>
+    <t>202.3 (29.6)</t>
+  </si>
+  <si>
+    <t>257.2 (44.5)</t>
+  </si>
+  <si>
+    <t>206.8 (31.3)</t>
+  </si>
+  <si>
+    <t>201.8 (31.8)</t>
+  </si>
+  <si>
+    <t>289.1 (47.3)</t>
+  </si>
+  <si>
+    <t>227.2 (39.9)</t>
+  </si>
+  <si>
+    <t>237.8 (46.7)</t>
+  </si>
+  <si>
+    <t>286.1 (53.1)</t>
+  </si>
+  <si>
+    <t>207.2 (34.2)</t>
+  </si>
+  <si>
+    <t>236.8 (41.9)</t>
+  </si>
+  <si>
+    <t>1.4 (3.2)</t>
+  </si>
+  <si>
+    <t>-9.8 (6.8)</t>
+  </si>
+  <si>
+    <t>-24.6 (7.9)</t>
+  </si>
+  <si>
+    <t>6.2 (5.1)</t>
+  </si>
+  <si>
+    <t>12.7 (8.0)</t>
+  </si>
+  <si>
+    <t>29.6 (11.3)</t>
+  </si>
+  <si>
+    <t>0.0 (3.4)</t>
+  </si>
+  <si>
+    <t>-7.4 (3.5)</t>
+  </si>
+  <si>
+    <t>-18.9 (8.9)</t>
+  </si>
+  <si>
+    <t>0.9 (2.8)</t>
+  </si>
+  <si>
+    <t>10.5 (6.0)</t>
+  </si>
+  <si>
+    <t>21.8 (12.6)</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>Latency (SD) in milliseconds</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="172" formatCode="\(##.#\)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -737,7 +1005,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -872,24 +1140,43 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2589,10 +2876,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:U28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15:N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2603,15 +2890,15 @@
     <col min="14" max="14" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C1" s="36" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C1" s="54" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C2" s="40" t="s">
         <v>30</v>
       </c>
@@ -2625,7 +2912,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B3" s="37"/>
       <c r="C3" s="37" t="s">
         <v>9</v>
@@ -2640,7 +2927,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B4" s="45" t="s">
         <v>62</v>
       </c>
@@ -2656,8 +2943,20 @@
       <c r="F4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P4" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>125</v>
+      </c>
+      <c r="R4" t="s">
+        <v>30</v>
+      </c>
+      <c r="S4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2674,8 +2973,17 @@
       <c r="F5" s="39" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="S5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T5" t="s">
+        <v>34</v>
+      </c>
+      <c r="U5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="C6" s="37" t="s">
         <v>9</v>
@@ -2689,8 +2997,23 @@
       <c r="F6" s="42" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q6" t="s">
+        <v>127</v>
+      </c>
+      <c r="R6" t="s">
+        <v>9</v>
+      </c>
+      <c r="S6" t="s">
+        <v>128</v>
+      </c>
+      <c r="T6" t="s">
+        <v>129</v>
+      </c>
+      <c r="U6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
         <v>63</v>
       </c>
@@ -2706,8 +3029,23 @@
       <c r="F7" s="42" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q7" t="s">
+        <v>62</v>
+      </c>
+      <c r="R7" t="s">
+        <v>32</v>
+      </c>
+      <c r="S7" t="s">
+        <v>131</v>
+      </c>
+      <c r="T7" t="s">
+        <v>132</v>
+      </c>
+      <c r="U7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="13"/>
       <c r="C8" s="38" t="s">
         <v>4</v>
@@ -2722,7 +3060,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B9" s="45"/>
       <c r="C9" s="37" t="s">
         <v>9</v>
@@ -2736,8 +3074,20 @@
       <c r="F9" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P9" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>127</v>
+      </c>
+      <c r="R9" t="s">
+        <v>4</v>
+      </c>
+      <c r="S9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B10" s="45" t="s">
         <v>62</v>
       </c>
@@ -2753,8 +3103,14 @@
       <c r="F10" s="42" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q10" t="s">
+        <v>133</v>
+      </c>
+      <c r="R10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -2772,7 +3128,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B12" s="13"/>
       <c r="C12" s="37" t="s">
         <v>9</v>
@@ -2786,8 +3142,20 @@
       <c r="F12" s="42" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="R12" t="s">
+        <v>9</v>
+      </c>
+      <c r="S12" t="s">
+        <v>136</v>
+      </c>
+      <c r="T12" t="s">
+        <v>137</v>
+      </c>
+      <c r="U12" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B13" s="13" t="s">
         <v>63</v>
       </c>
@@ -2803,8 +3171,23 @@
       <c r="F13" s="42" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q13" t="s">
+        <v>63</v>
+      </c>
+      <c r="R13" t="s">
+        <v>32</v>
+      </c>
+      <c r="S13" t="s">
+        <v>139</v>
+      </c>
+      <c r="T13" t="s">
+        <v>140</v>
+      </c>
+      <c r="U13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C14" s="37" t="s">
         <v>4</v>
       </c>
@@ -2817,26 +3200,42 @@
       <c r="F14" s="42" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H15" s="52"/>
-      <c r="I15" s="53"/>
-      <c r="J15" s="54" t="s">
-        <v>73</v>
-      </c>
-      <c r="K15" s="54"/>
-      <c r="L15" s="54"/>
-      <c r="M15" s="54"/>
-      <c r="N15" s="55" t="s">
+      <c r="R14" t="s">
+        <v>4</v>
+      </c>
+      <c r="S14" t="s">
+        <v>142</v>
+      </c>
+      <c r="T14" t="s">
+        <v>143</v>
+      </c>
+      <c r="U14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="H15" s="57" t="s">
+        <v>124</v>
+      </c>
+      <c r="I15" s="52" t="s">
+        <v>125</v>
+      </c>
+      <c r="J15" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="K15" s="55" t="s">
+        <v>212</v>
+      </c>
+      <c r="L15" s="55"/>
+      <c r="M15" s="55"/>
+      <c r="N15" s="58" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H16" s="47"/>
-      <c r="I16" s="43"/>
-      <c r="J16" s="5" t="s">
-        <v>74</v>
-      </c>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="H16" s="59"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
       <c r="K16" s="5" t="s">
         <v>33</v>
       </c>
@@ -2846,254 +3245,344 @@
       <c r="M16" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="N16" s="56" t="s">
+      <c r="N16" s="53" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="17" spans="8:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="H17" s="47"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="43" t="s">
+      <c r="Q16" t="s">
+        <v>127</v>
+      </c>
+      <c r="R16" t="s">
         <v>9</v>
       </c>
-      <c r="K17" s="43" t="s">
-        <v>75</v>
-      </c>
-      <c r="L17" s="43" t="s">
-        <v>87</v>
-      </c>
-      <c r="M17" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="N17" s="57" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="18" spans="8:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="H18" s="47"/>
+      <c r="S16" t="s">
+        <v>145</v>
+      </c>
+      <c r="T16" t="s">
+        <v>146</v>
+      </c>
+      <c r="U16" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="17" spans="4:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H17" s="59"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="M17" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="N17" s="53" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>62</v>
+      </c>
+      <c r="R17" t="s">
+        <v>32</v>
+      </c>
+      <c r="S17" t="s">
+        <v>148</v>
+      </c>
+      <c r="T17" t="s">
+        <v>149</v>
+      </c>
+      <c r="U17" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D18" s="56">
+        <v>24</v>
+      </c>
+      <c r="H18" s="59"/>
       <c r="I18" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="J18" s="43" t="s">
+      <c r="J18" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K18" s="43" t="s">
-        <v>76</v>
-      </c>
-      <c r="L18" s="42" t="s">
-        <v>88</v>
-      </c>
-      <c r="M18" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="N18" s="58" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="19" spans="8:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="H19" s="47" t="s">
+      <c r="K18" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="L18" s="50" t="s">
+        <v>176</v>
+      </c>
+      <c r="M18" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="N18" s="60" t="s">
+        <v>200</v>
+      </c>
+      <c r="P18" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>127</v>
+      </c>
+      <c r="R18" t="s">
+        <v>4</v>
+      </c>
+      <c r="S18" t="s">
+        <v>151</v>
+      </c>
+      <c r="T18" t="s">
+        <v>152</v>
+      </c>
+      <c r="U18" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="H19" s="59" t="s">
         <v>6</v>
       </c>
       <c r="I19" s="5"/>
-      <c r="J19" s="43" t="s">
+      <c r="J19" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K19" s="42" t="s">
-        <v>77</v>
-      </c>
-      <c r="L19" s="42" t="s">
-        <v>89</v>
-      </c>
-      <c r="M19" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="N19" s="58" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="20" spans="8:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="H20" s="47"/>
+      <c r="K19" s="50" t="s">
+        <v>165</v>
+      </c>
+      <c r="L19" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="M19" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="N19" s="60" t="s">
+        <v>201</v>
+      </c>
+      <c r="R19" t="s">
+        <v>9</v>
+      </c>
+      <c r="S19" t="s">
+        <v>154</v>
+      </c>
+      <c r="T19" t="s">
+        <v>155</v>
+      </c>
+      <c r="U19" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="20" spans="4:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H20" s="59"/>
       <c r="I20" s="5"/>
-      <c r="J20" s="43" t="s">
+      <c r="J20" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K20" s="42" t="s">
-        <v>78</v>
-      </c>
-      <c r="L20" s="42" t="s">
-        <v>90</v>
-      </c>
-      <c r="M20" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="N20" s="57" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="21" spans="8:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="H21" s="47"/>
+      <c r="K20" s="50" t="s">
+        <v>166</v>
+      </c>
+      <c r="L20" s="50" t="s">
+        <v>177</v>
+      </c>
+      <c r="M20" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="N20" s="53" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>63</v>
+      </c>
+      <c r="R20" t="s">
+        <v>32</v>
+      </c>
+      <c r="S20" t="s">
+        <v>157</v>
+      </c>
+      <c r="T20" t="s">
+        <v>158</v>
+      </c>
+      <c r="U20" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="21" spans="4:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H21" s="59"/>
       <c r="I21" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="J21" s="43" t="s">
+      <c r="J21" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K21" s="42" t="s">
-        <v>79</v>
-      </c>
-      <c r="L21" s="42" t="s">
-        <v>91</v>
-      </c>
-      <c r="M21" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="N21" s="57" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="22" spans="8:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="H22" s="47"/>
+      <c r="K21" s="50" t="s">
+        <v>167</v>
+      </c>
+      <c r="L21" s="50" t="s">
+        <v>178</v>
+      </c>
+      <c r="M21" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="N21" s="53" t="s">
+        <v>203</v>
+      </c>
+      <c r="R21" t="s">
+        <v>4</v>
+      </c>
+      <c r="S21" t="s">
+        <v>160</v>
+      </c>
+      <c r="T21" t="s">
+        <v>161</v>
+      </c>
+      <c r="U21" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="22" spans="4:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H22" s="59"/>
       <c r="I22" s="5"/>
-      <c r="J22" s="43" t="s">
+      <c r="J22" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K22" s="42" t="s">
-        <v>80</v>
-      </c>
-      <c r="L22" s="42" t="s">
-        <v>92</v>
-      </c>
-      <c r="M22" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="N22" s="57" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="23" spans="8:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="H23" s="47"/>
+      <c r="K22" s="50" t="s">
+        <v>168</v>
+      </c>
+      <c r="L22" s="50" t="s">
+        <v>179</v>
+      </c>
+      <c r="M22" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="N22" s="53" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="23" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="H23" s="59"/>
       <c r="I23" s="5"/>
-      <c r="J23" s="43" t="s">
+      <c r="J23" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K23" s="42" t="s">
-        <v>81</v>
-      </c>
-      <c r="L23" s="42" t="s">
-        <v>93</v>
-      </c>
-      <c r="M23" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="N23" s="57" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="24" spans="8:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="H24" s="47"/>
+      <c r="K23" s="50" t="s">
+        <v>169</v>
+      </c>
+      <c r="L23" s="50" t="s">
+        <v>180</v>
+      </c>
+      <c r="M23" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="N23" s="53" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="24" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="H24" s="59"/>
       <c r="I24" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="J24" s="43" t="s">
+      <c r="J24" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K24" s="42" t="s">
-        <v>82</v>
-      </c>
-      <c r="L24" s="42" t="s">
-        <v>94</v>
-      </c>
-      <c r="M24" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="N24" s="58" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="25" spans="8:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="H25" s="47" t="s">
+      <c r="K24" s="50" t="s">
+        <v>170</v>
+      </c>
+      <c r="L24" s="50" t="s">
+        <v>181</v>
+      </c>
+      <c r="M24" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="N24" s="60" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="25" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="H25" s="59" t="s">
         <v>5</v>
       </c>
       <c r="I25" s="5"/>
-      <c r="J25" s="43" t="s">
+      <c r="J25" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K25" s="42" t="s">
-        <v>83</v>
-      </c>
-      <c r="L25" s="42" t="s">
-        <v>95</v>
-      </c>
-      <c r="M25" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="N25" s="58" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="26" spans="8:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="H26" s="47"/>
+      <c r="K25" s="50" t="s">
+        <v>171</v>
+      </c>
+      <c r="L25" s="50" t="s">
+        <v>182</v>
+      </c>
+      <c r="M25" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="N25" s="60" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="26" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="H26" s="59"/>
       <c r="I26" s="5"/>
-      <c r="J26" s="43" t="s">
+      <c r="J26" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K26" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="L26" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="M26" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="N26" s="57" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="27" spans="8:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="H27" s="47"/>
+      <c r="K26" s="50" t="s">
+        <v>172</v>
+      </c>
+      <c r="L26" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="M26" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="N26" s="53" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="27" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="H27" s="59"/>
       <c r="I27" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="J27" s="43" t="s">
+      <c r="J27" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K27" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="L27" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="M27" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="N27" s="57" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="28" spans="8:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="H28" s="59"/>
-      <c r="I28" s="60"/>
-      <c r="J28" s="60" t="s">
+      <c r="K27" s="50" t="s">
+        <v>173</v>
+      </c>
+      <c r="L27" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="M27" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="N27" s="53" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="28" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="H28" s="61"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="K28" s="61" t="s">
-        <v>86</v>
-      </c>
-      <c r="L28" s="62" t="s">
-        <v>98</v>
-      </c>
-      <c r="M28" s="62" t="s">
-        <v>110</v>
-      </c>
-      <c r="N28" s="63" t="s">
-        <v>123</v>
+      <c r="K28" s="62" t="s">
+        <v>174</v>
+      </c>
+      <c r="L28" s="63" t="s">
+        <v>185</v>
+      </c>
+      <c r="M28" s="63" t="s">
+        <v>198</v>
+      </c>
+      <c r="N28" s="64" t="s">
+        <v>210</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C1:F1"/>
-    <mergeCell ref="J15:M15"/>
+    <mergeCell ref="K15:M15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3103,8 +3592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:G40"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3406,14 +3895,20 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>124</v>
+      </c>
+      <c r="B12" t="s">
+        <v>125</v>
+      </c>
       <c r="C12" s="40" t="s">
         <v>30</v>
       </c>
@@ -3763,12 +4258,12 @@
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C27" s="36" t="s">
+      <c r="C27" s="54" t="s">
         <v>73</v>
       </c>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="54"/>
       <c r="G27" t="s">
         <v>34</v>
       </c>
@@ -4425,6 +4920,7 @@
     <mergeCell ref="C27:F27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>